<commit_message>
Updated wind_cost to include more accurate capital costs, height cost adders, and formula for cost projections
</commit_message>
<xml_diff>
--- a/data_share/WIND_HEIGHTS_COSTS_20140320.xlsx
+++ b/data_share/WIND_HEIGHTS_COSTS_20140320.xlsx
@@ -14,8 +14,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ben Sigrin - NREL</author>
+  </authors>
+  <commentList>
+    <comment ref="U7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Sigrin - NREL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The original reference height was 14m. However, with height adders, it was giving $12/W installed cost fro 2.5kW at 30m. Judgement call to not add adders here</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>Turbines 20 kW</t>
   </si>
@@ -134,15 +168,9 @@
     <t>Values to Use in DW Model</t>
   </si>
   <si>
-    <t>From Data</t>
-  </si>
-  <si>
     <t>size (kW)</t>
   </si>
   <si>
-    <t>Model (proposed)</t>
-  </si>
-  <si>
     <t>h1</t>
   </si>
   <si>
@@ -165,19 +193,42 @@
   </si>
   <si>
     <t>fit</t>
+  </si>
+  <si>
+    <t>Wind Turbine Costs and Height Adders</t>
+  </si>
+  <si>
+    <t>Default Height</t>
+  </si>
+  <si>
+    <t>Original Data</t>
+  </si>
+  <si>
+    <t>For Regression</t>
+  </si>
+  <si>
+    <t>Values for Model</t>
+  </si>
+  <si>
+    <t>Cost At Reference Height ($/kW)</t>
+  </si>
+  <si>
+    <t>Adj. Height Cost Adder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0\ &quot;kW&quot;"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,8 +260,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +298,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -464,7 +542,12 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,11 +673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="179176192"/>
-        <c:axId val="179177728"/>
+        <c:axId val="51703808"/>
+        <c:axId val="51705344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="179176192"/>
+        <c:axId val="51703808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,12 +687,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179177728"/>
+        <c:crossAx val="51705344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="179177728"/>
+        <c:axId val="51705344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,7 +703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179176192"/>
+        <c:crossAx val="51703808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -634,6 +717,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:ln>
@@ -682,7 +766,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.6609494914053177E-2"/>
+          <c:y val="0.12534274368518949"/>
+          <c:w val="0.90467212240671746"/>
+          <c:h val="0.80003213405294848"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -691,7 +785,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TO_MODEL!$K$3</c:f>
+              <c:f>TO_MODEL!$K$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -716,7 +810,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>TO_MODEL!$J$4:$J$13</c:f>
+              <c:f>TO_MODEL!$J$7:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -755,7 +849,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TO_MODEL!$K$4:$K$13</c:f>
+              <c:f>TO_MODEL!$K$7:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -802,11 +896,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="180891008"/>
-        <c:axId val="180892800"/>
+        <c:axId val="51779840"/>
+        <c:axId val="51781632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="180891008"/>
+        <c:axId val="51779840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -816,30 +910,38 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180892800"/>
+        <c:crossAx val="51781632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="180892800"/>
+        <c:axId val="51781632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180891008"/>
+        <c:crossAx val="51779840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46136899172007168"/>
+          <c:y val="0.16459507574957957"/>
+          <c:w val="0.33435693735845368"/>
+          <c:h val="0.20287923642979525"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -874,7 +976,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10052156473371529"/>
+          <c:y val="0.18890037735182091"/>
+          <c:w val="0.85216573724280409"/>
+          <c:h val="0.69863428687575668"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -883,7 +995,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TO_MODEL!$P$3</c:f>
+              <c:f>TO_MODEL!$P$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -902,13 +1014,18 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.29871600931490166"/>
+                  <c:y val="-0.37484664416947883"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(TO_MODEL!$J$4:$J$6,TO_MODEL!$J$9,TO_MODEL!$J$13)</c:f>
+              <c:f>(TO_MODEL!$J$7:$J$9,TO_MODEL!$J$12,TO_MODEL!$J$16)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -932,7 +1049,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(TO_MODEL!$P$4:$P$6,TO_MODEL!$P$9,TO_MODEL!$P$13)</c:f>
+              <c:f>(TO_MODEL!$P$7:$P$9,TO_MODEL!$P$12,TO_MODEL!$P$16)</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -964,11 +1081,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="180917760"/>
-        <c:axId val="180919296"/>
+        <c:axId val="51798784"/>
+        <c:axId val="51800320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="180917760"/>
+        <c:axId val="51798784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -978,23 +1095,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180919296"/>
+        <c:crossAx val="51800320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="180919296"/>
+        <c:axId val="51800320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180917760"/>
+        <c:crossAx val="51798784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1065,7 +1181,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.10015507436570428"/>
           <c:y val="0.19480351414406533"/>
-          <c:w val="0.52363538932633424"/>
+          <c:w val="0.84931380445920246"/>
           <c:h val="0.68921660834062404"/>
         </c:manualLayout>
       </c:layout>
@@ -1077,7 +1193,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TO_MODEL!$P$3</c:f>
+              <c:f>TO_MODEL!$P$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1107,7 +1223,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(TO_MODEL!$J$4:$J$6,TO_MODEL!$J$9)</c:f>
+              <c:f>(TO_MODEL!$J$7:$J$9,TO_MODEL!$J$12)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1128,7 +1244,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(TO_MODEL!$P$4:$P$6,TO_MODEL!$P$9)</c:f>
+              <c:f>(TO_MODEL!$P$7:$P$9,TO_MODEL!$P$12)</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1157,11 +1273,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="180957184"/>
-        <c:axId val="180958720"/>
+        <c:axId val="51817472"/>
+        <c:axId val="54280960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="180957184"/>
+        <c:axId val="51817472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,23 +1287,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180958720"/>
+        <c:crossAx val="54280960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="180958720"/>
+        <c:axId val="54280960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180957184"/>
+        <c:crossAx val="51817472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1205,8 +1320,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66713757655293093"/>
-          <c:y val="0.22834098862642174"/>
+          <c:x val="0.60868256812366095"/>
+          <c:y val="0.22834098862642169"/>
           <c:w val="0.30230686789151356"/>
           <c:h val="0.27931321084864391"/>
         </c:manualLayout>
@@ -1274,7 +1389,7 @@
           <c:yMode val="edge"/>
           <c:x val="9.3085739282589675E-2"/>
           <c:y val="0.19480351414406533"/>
-          <c:w val="0.54588517060367459"/>
+          <c:w val="0.8554597385428091"/>
           <c:h val="0.68921660834062404"/>
         </c:manualLayout>
       </c:layout>
@@ -1286,7 +1401,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TO_MODEL!$P$3</c:f>
+              <c:f>TO_MODEL!$P$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1307,8 +1422,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.8458005249343835E-2"/>
-                  <c:y val="0.11913531641878099"/>
+                  <c:x val="-0.52767575824001312"/>
+                  <c:y val="4.969087197433654E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1316,7 +1431,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(TO_MODEL!$J$9,TO_MODEL!$J$13)</c:f>
+              <c:f>(TO_MODEL!$J$12,TO_MODEL!$J$16)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1331,7 +1446,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(TO_MODEL!$P$9,TO_MODEL!$P$13)</c:f>
+              <c:f>(TO_MODEL!$P$12,TO_MODEL!$P$16)</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1354,11 +1469,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="180971776"/>
-        <c:axId val="180977664"/>
+        <c:axId val="54306304"/>
+        <c:axId val="54307840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="180971776"/>
+        <c:axId val="54306304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1368,23 +1483,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180977664"/>
+        <c:crossAx val="54307840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="180977664"/>
+        <c:axId val="54307840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:numFmt formatCode="&quot;$&quot;#,##0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180971776"/>
+        <c:crossAx val="54306304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1402,8 +1516,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.70324868766404203"/>
-          <c:y val="0.43204469233012538"/>
+          <c:x val="0.6440653784572854"/>
+          <c:y val="0.56167432195975509"/>
           <c:w val="0.28008464566929137"/>
           <c:h val="0.27931321084864391"/>
         </c:manualLayout>
@@ -1417,6 +1531,180 @@
         </a:ln>
       </c:spPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TO_MODEL!$S$7:$S$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0\ "kW"</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TO_MODEL!$Y$7:$Y$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>8780</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7790</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7362.7896483463155</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6449.2642045483453</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5395.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4131.8212120402559</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3278</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2387.8230161497218</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0">
+                  <c:v>2145</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1810</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1810</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="56552448"/>
+        <c:axId val="56550912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="56552448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0\ &quot;kW&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56550912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="56550912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56552448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1562,15 +1850,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>24765</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>60485</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>107157</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>148591</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1591,16 +1879,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>166689</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>433387</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>773906</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>71439</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1621,16 +1909,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>223837</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>452437</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1651,16 +1939,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>423862</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>547689</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>30956</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1674,6 +1962,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>110729</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>881062</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1971,7 +2289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y702"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -3524,11 +3842,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3541,461 +3859,760 @@
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="16" max="16" width="10.28515625" customWidth="1"/>
     <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="19" max="19" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.5703125" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" s="40" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="40" t="s">
+    <row r="2" spans="2:25" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" s="40" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="S5" s="40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" s="39" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="K6" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="39" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="2:20" s="39" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="s">
+      <c r="N6" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="T6" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="39" t="s">
+      <c r="U6" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="39" t="s">
+      <c r="V6" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="W6" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="X6" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y6" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7" s="41">
+        <v>230</v>
+      </c>
+      <c r="H7" s="41">
+        <v>550</v>
+      </c>
+      <c r="J7">
+        <v>2.5</v>
+      </c>
+      <c r="K7">
+        <f>C7</f>
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="P7" s="47">
+        <v>230</v>
+      </c>
+      <c r="Q7" s="45">
+        <f>LN(P7)</f>
+        <v>5.4380793089231956</v>
+      </c>
+      <c r="S7" s="49">
+        <v>2.5</v>
+      </c>
+      <c r="T7">
+        <v>8780</v>
+      </c>
+      <c r="U7">
+        <v>30</v>
+      </c>
+      <c r="V7">
+        <v>30</v>
+      </c>
+      <c r="W7">
+        <v>230</v>
+      </c>
+      <c r="X7">
+        <f>(V7-U7)*W7</f>
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <f>T7+X7</f>
+        <v>8780</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>7.79</v>
+      </c>
+      <c r="D8">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>37</v>
+      </c>
+      <c r="G8" s="41">
+        <v>130</v>
+      </c>
+      <c r="H8" s="41"/>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8:K16" si="0">C8</f>
+        <v>7.79</v>
+      </c>
+      <c r="L8">
+        <v>30</v>
+      </c>
+      <c r="M8">
         <v>40</v>
       </c>
-      <c r="K3" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="39" t="s">
+      <c r="P8" s="47">
+        <v>130</v>
+      </c>
+      <c r="Q8" s="45">
+        <f t="shared" ref="Q8:Q9" si="1">LN(P8)</f>
+        <v>4.8675344504555822</v>
+      </c>
+      <c r="S8" s="49">
+        <v>5</v>
+      </c>
+      <c r="T8">
+        <v>7790</v>
+      </c>
+      <c r="U8">
+        <v>30</v>
+      </c>
+      <c r="V8">
+        <v>30</v>
+      </c>
+      <c r="W8">
+        <v>130</v>
+      </c>
+      <c r="X8">
+        <f t="shared" ref="X8:X17" si="2">(V8-U8)*W8</f>
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" ref="Y8:Y17" si="3">T8+X8</f>
+        <v>7790</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>7.64</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>37</v>
+      </c>
+      <c r="F9">
         <v>43</v>
       </c>
-      <c r="N3" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>8.7799999999999994</v>
-      </c>
-      <c r="D4">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>30</v>
-      </c>
-      <c r="G4" s="41">
-        <v>230</v>
-      </c>
-      <c r="H4" s="41">
-        <v>550</v>
-      </c>
-      <c r="J4">
-        <v>2.5</v>
-      </c>
-      <c r="K4">
-        <f>C4</f>
-        <v>8.7799999999999994</v>
-      </c>
-      <c r="L4">
-        <v>30</v>
-      </c>
-      <c r="P4" s="47">
-        <v>230</v>
-      </c>
-      <c r="Q4" s="45">
-        <f>LN(P4)</f>
-        <v>5.4380793089231956</v>
-      </c>
-      <c r="T4" s="48">
-        <f>J4*K4*1000</f>
-        <v>21950</v>
-      </c>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>7.79</v>
-      </c>
-      <c r="D5">
-        <v>24</v>
-      </c>
-      <c r="E5">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>37</v>
-      </c>
-      <c r="G5" s="41">
-        <v>130</v>
-      </c>
-      <c r="H5" s="41"/>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ref="K5:K13" si="0">C5</f>
-        <v>7.79</v>
-      </c>
-      <c r="L5">
-        <v>30</v>
-      </c>
-      <c r="M5">
-        <v>40</v>
-      </c>
-      <c r="P5" s="47">
-        <v>130</v>
-      </c>
-      <c r="Q5" s="45">
-        <f t="shared" ref="Q5:Q6" si="1">LN(P5)</f>
-        <v>4.8675344504555822</v>
-      </c>
-      <c r="T5" s="48">
-        <f>P4*2.5*10</f>
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>7.64</v>
-      </c>
-      <c r="D6">
-        <v>30</v>
-      </c>
-      <c r="E6">
-        <v>37</v>
-      </c>
-      <c r="F6">
-        <v>43</v>
-      </c>
-      <c r="G6" s="41">
+      <c r="G9" s="41">
         <v>80</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H9" s="41">
         <v>800</v>
       </c>
-      <c r="J6">
+      <c r="J9">
         <v>10</v>
       </c>
-      <c r="K6">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>7.64</v>
       </c>
-      <c r="L6">
+      <c r="L9">
         <v>30</v>
       </c>
-      <c r="M6">
+      <c r="M9">
         <v>40</v>
       </c>
-      <c r="N6">
+      <c r="N9" s="50">
         <v>50</v>
       </c>
-      <c r="P6" s="47">
+      <c r="P9" s="47">
         <v>80</v>
       </c>
-      <c r="Q6" s="45">
+      <c r="Q9" s="45">
         <f t="shared" si="1"/>
         <v>4.3820266346738812</v>
       </c>
-      <c r="T6" s="47"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="S9" s="49">
+        <v>10</v>
+      </c>
+      <c r="T9">
+        <v>7640</v>
+      </c>
+      <c r="U9">
+        <v>33</v>
+      </c>
+      <c r="V9">
+        <v>30</v>
+      </c>
+      <c r="W9">
+        <v>80</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="2"/>
+        <v>-240</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="3"/>
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>7.25</v>
       </c>
-      <c r="D7">
+      <c r="D10">
         <v>30</v>
       </c>
-      <c r="E7">
+      <c r="E10">
         <v>37</v>
       </c>
-      <c r="F7">
+      <c r="F10">
         <v>43</v>
-      </c>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="J7">
-        <v>20</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>7.25</v>
-      </c>
-      <c r="L7">
-        <v>30</v>
-      </c>
-      <c r="M7">
-        <v>40</v>
-      </c>
-      <c r="N7">
-        <v>50</v>
-      </c>
-      <c r="P7" s="43">
-        <f>564*J7^-0.904</f>
-        <v>37.596549448771725</v>
-      </c>
-      <c r="Q7" s="45"/>
-      <c r="T7" s="47"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>6.4</v>
-      </c>
-      <c r="D8">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>37</v>
-      </c>
-      <c r="F8">
-        <v>43</v>
-      </c>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="J8">
-        <v>50</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>6.4</v>
-      </c>
-      <c r="L8">
-        <v>30</v>
-      </c>
-      <c r="M8">
-        <v>40</v>
-      </c>
-      <c r="N8">
-        <v>50</v>
-      </c>
-      <c r="P8" s="43">
-        <f>564*J8^-0.904</f>
-        <v>16.421401516114997</v>
-      </c>
-      <c r="Q8" s="45"/>
-      <c r="T8" s="47"/>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>5.37</v>
-      </c>
-      <c r="D9">
-        <v>37</v>
-      </c>
-      <c r="E9">
-        <v>37</v>
-      </c>
-      <c r="F9">
-        <v>50</v>
-      </c>
-      <c r="G9" s="42">
-        <v>8.4</v>
-      </c>
-      <c r="H9" s="41">
-        <v>840</v>
-      </c>
-      <c r="J9">
-        <v>100</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>5.37</v>
-      </c>
-      <c r="M9">
-        <v>40</v>
-      </c>
-      <c r="N9">
-        <v>50</v>
-      </c>
-      <c r="P9" s="48">
-        <v>8.4</v>
-      </c>
-      <c r="Q9" s="45">
-        <f>LN(P9)</f>
-        <v>2.1282317058492679</v>
-      </c>
-      <c r="T9" s="49"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>2.48</v>
       </c>
       <c r="G10" s="41"/>
       <c r="H10" s="41"/>
       <c r="J10">
-        <v>250</v>
-      </c>
-      <c r="K10" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="N10">
+        <v>20</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>7.25</v>
+      </c>
+      <c r="L10">
+        <v>30</v>
+      </c>
+      <c r="M10">
+        <v>40</v>
+      </c>
+      <c r="N10" s="50">
         <v>50</v>
       </c>
-      <c r="P10" s="44">
-        <f>17.26*J10^-0.156</f>
-        <v>7.2939393877120153</v>
+      <c r="P10" s="43">
+        <f>564*J10^-0.904</f>
+        <v>37.596549448771725</v>
       </c>
       <c r="Q10" s="45"/>
-      <c r="T10" s="48"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S10" s="49">
+        <v>20</v>
+      </c>
+      <c r="T10">
+        <v>7250</v>
+      </c>
+      <c r="U10">
+        <v>37</v>
+      </c>
+      <c r="V10">
+        <v>40</v>
+      </c>
+      <c r="W10">
+        <v>37.596549448771725</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="2"/>
+        <v>112.78964834631518</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="3"/>
+        <v>7362.7896483463155</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>6.4</v>
       </c>
       <c r="D11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E11">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F11">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="G11" s="41"/>
       <c r="H11" s="41"/>
       <c r="J11">
-        <v>500</v>
-      </c>
-      <c r="K11" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="N11">
         <v>50</v>
       </c>
-      <c r="O11">
-        <v>80</v>
-      </c>
-      <c r="P11" s="44">
-        <f t="shared" ref="P11:P12" si="2">17.26*J11^-0.156</f>
-        <v>6.5463839094293448</v>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>6.4</v>
+      </c>
+      <c r="L11">
+        <v>30</v>
+      </c>
+      <c r="M11">
+        <v>40</v>
+      </c>
+      <c r="N11" s="50">
+        <v>50</v>
+      </c>
+      <c r="P11" s="43">
+        <f>564*J11^-0.904</f>
+        <v>16.421401516114997</v>
       </c>
       <c r="Q11" s="45"/>
-      <c r="T11" s="48"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S11" s="49">
+        <v>50</v>
+      </c>
+      <c r="T11">
+        <v>6400</v>
+      </c>
+      <c r="U11">
+        <v>37</v>
+      </c>
+      <c r="V11">
+        <v>40</v>
+      </c>
+      <c r="W11">
+        <v>16.421401516114997</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="2"/>
+        <v>49.264204548344992</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="3"/>
+        <v>6449.2642045483453</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>5.37</v>
       </c>
       <c r="D12">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E12">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="F12">
-        <v>80</v>
-      </c>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
+        <v>50</v>
+      </c>
+      <c r="G12" s="42">
+        <v>8.4</v>
+      </c>
+      <c r="H12" s="41">
+        <v>840</v>
+      </c>
       <c r="J12">
-        <v>750</v>
+        <v>100</v>
       </c>
       <c r="K12">
-        <f>C10</f>
-        <v>2.48</v>
+        <f t="shared" si="0"/>
+        <v>5.37</v>
+      </c>
+      <c r="M12">
+        <v>40</v>
       </c>
       <c r="N12">
         <v>50</v>
       </c>
-      <c r="O12">
-        <v>80</v>
-      </c>
-      <c r="P12" s="44">
+      <c r="P12" s="48">
+        <v>8.4</v>
+      </c>
+      <c r="Q12" s="45">
+        <f>LN(P12)</f>
+        <v>2.1282317058492679</v>
+      </c>
+      <c r="S12" s="49">
+        <v>100</v>
+      </c>
+      <c r="T12">
+        <v>5370</v>
+      </c>
+      <c r="U12">
+        <v>37</v>
+      </c>
+      <c r="V12">
+        <v>40</v>
+      </c>
+      <c r="W12">
+        <v>8.4</v>
+      </c>
+      <c r="X12">
         <f t="shared" si="2"/>
-        <v>6.1451322566852165</v>
-      </c>
-      <c r="Q12" s="45"/>
-      <c r="T12" s="48"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+        <v>25.200000000000003</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="3"/>
+        <v>5395.2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>1.81</v>
-      </c>
-      <c r="D13">
-        <v>70</v>
-      </c>
-      <c r="E13">
-        <v>80</v>
-      </c>
-      <c r="F13">
-        <v>100</v>
-      </c>
-      <c r="G13" s="42">
-        <v>5.5</v>
-      </c>
+        <v>2.48</v>
+      </c>
+      <c r="G13" s="41"/>
       <c r="H13" s="41"/>
       <c r="J13">
+        <v>250</v>
+      </c>
+      <c r="K13" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13">
+        <v>50</v>
+      </c>
+      <c r="P13" s="44">
+        <f>17.26*J13^-0.156</f>
+        <v>7.2939393877120153</v>
+      </c>
+      <c r="Q13" s="45"/>
+      <c r="S13" s="49">
+        <v>250</v>
+      </c>
+      <c r="T13">
+        <v>4037</v>
+      </c>
+      <c r="U13">
+        <v>37</v>
+      </c>
+      <c r="V13">
+        <v>50</v>
+      </c>
+      <c r="W13">
+        <v>7.2939393877120153</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="2"/>
+        <v>94.821212040256199</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="3"/>
+        <v>4131.8212120402559</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <v>70</v>
+      </c>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="J14">
+        <v>500</v>
+      </c>
+      <c r="K14" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14">
+        <v>50</v>
+      </c>
+      <c r="O14">
+        <v>80</v>
+      </c>
+      <c r="P14" s="44">
+        <f t="shared" ref="P14:P15" si="4">17.26*J14^-0.156</f>
+        <v>6.5463839094293448</v>
+      </c>
+      <c r="Q14" s="45"/>
+      <c r="S14" s="49">
+        <v>500</v>
+      </c>
+      <c r="T14">
+        <v>3278</v>
+      </c>
+      <c r="U14">
+        <v>50</v>
+      </c>
+      <c r="V14">
+        <v>50</v>
+      </c>
+      <c r="W14">
+        <v>6.5463839094293448</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="3"/>
+        <v>3278</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>65</v>
+      </c>
+      <c r="F15">
+        <v>80</v>
+      </c>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="J15">
+        <v>750</v>
+      </c>
+      <c r="K15">
+        <f>C13</f>
+        <v>2.48</v>
+      </c>
+      <c r="N15">
+        <v>50</v>
+      </c>
+      <c r="O15">
+        <v>80</v>
+      </c>
+      <c r="P15" s="44">
+        <f t="shared" si="4"/>
+        <v>6.1451322566852165</v>
+      </c>
+      <c r="Q15" s="45"/>
+      <c r="S15" s="49">
+        <v>750</v>
+      </c>
+      <c r="T15">
+        <v>2480</v>
+      </c>
+      <c r="U15">
+        <v>65</v>
+      </c>
+      <c r="V15">
+        <v>50</v>
+      </c>
+      <c r="W15">
+        <v>6.1451322566852165</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="2"/>
+        <v>-92.176983850278248</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="3"/>
+        <v>2387.8230161497218</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>1.81</v>
+      </c>
+      <c r="D16">
+        <v>70</v>
+      </c>
+      <c r="E16">
+        <v>80</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="G16" s="42">
+        <v>5.5</v>
+      </c>
+      <c r="H16" s="41"/>
+      <c r="J16">
         <v>1500</v>
       </c>
-      <c r="K13">
+      <c r="K16">
         <f t="shared" si="0"/>
         <v>1.81</v>
       </c>
-      <c r="O13">
+      <c r="O16">
         <v>80</v>
       </c>
-      <c r="P13" s="48">
+      <c r="P16" s="48">
         <v>5.5</v>
       </c>
-      <c r="Q13" s="45">
-        <f>LN(P13)</f>
+      <c r="Q16" s="45">
+        <f>LN(P16)</f>
         <v>1.7047480922384253</v>
+      </c>
+      <c r="S16" s="52">
+        <v>1000</v>
+      </c>
+      <c r="T16">
+        <v>2145</v>
+      </c>
+      <c r="U16">
+        <v>80</v>
+      </c>
+      <c r="V16">
+        <v>80</v>
+      </c>
+      <c r="W16" s="53">
+        <v>5.8230000000000004</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="54">
+        <f>T16</f>
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="17" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S17" s="49">
+        <v>1500</v>
+      </c>
+      <c r="T17">
+        <v>1810</v>
+      </c>
+      <c r="U17">
+        <v>80</v>
+      </c>
+      <c r="V17">
+        <v>80</v>
+      </c>
+      <c r="W17">
+        <v>5.5</v>
+      </c>
+      <c r="X17">
+        <f>(V17-U17)*W17</f>
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <f>T17+X17</f>
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="18" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S18" s="49">
+        <f>3000</f>
+        <v>3000</v>
+      </c>
+      <c r="T18">
+        <v>1810</v>
+      </c>
+      <c r="U18">
+        <v>80</v>
+      </c>
+      <c r="V18">
+        <v>80</v>
+      </c>
+      <c r="W18">
+        <v>5.5</v>
+      </c>
+      <c r="X18">
+        <f>(V18-U18)*W18</f>
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <f>T18+X18</f>
+        <v>1810</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added script to automate creation of R markdown file
Added calculation of LCOE
</commit_message>
<xml_diff>
--- a/data_share/WIND_HEIGHTS_COSTS_20140320.xlsx
+++ b/data_share/WIND_HEIGHTS_COSTS_20140320.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="105" windowWidth="22110" windowHeight="9135" activeTab="1"/>
+    <workbookView xWindow="30" yWindow="165" windowWidth="22110" windowHeight="9075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Values to Use in DW Diffusion" sheetId="11" r:id="rId1"/>
@@ -213,7 +213,7 @@
     <t>Cost At Reference Height ($/kW)</t>
   </si>
   <si>
-    <t>Adj. Height Cost Adder</t>
+    <t>Adj. Height Cost Adder ($/kW)</t>
   </si>
 </sst>
 </file>
@@ -226,7 +226,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.0"/>
     <numFmt numFmtId="168" formatCode="0.0\ &quot;kW&quot;"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.000"/>
+    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -282,7 +282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,8 +307,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -408,11 +414,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -542,12 +628,29 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,11 +776,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51703808"/>
-        <c:axId val="51705344"/>
+        <c:axId val="146222464"/>
+        <c:axId val="146793984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51703808"/>
+        <c:axId val="146222464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,12 +790,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51705344"/>
+        <c:crossAx val="146793984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51705344"/>
+        <c:axId val="146793984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -703,7 +806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51703808"/>
+        <c:crossAx val="146222464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -717,7 +820,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:ln>
@@ -896,11 +998,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51779840"/>
-        <c:axId val="51781632"/>
+        <c:axId val="62745984"/>
+        <c:axId val="62760064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51779840"/>
+        <c:axId val="62745984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,12 +1012,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51781632"/>
+        <c:crossAx val="62760064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51781632"/>
+        <c:axId val="62760064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -925,7 +1027,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51779840"/>
+        <c:crossAx val="62745984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1081,11 +1183,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51798784"/>
-        <c:axId val="51800320"/>
+        <c:axId val="62782848"/>
+        <c:axId val="62919808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51798784"/>
+        <c:axId val="62782848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,12 +1197,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51800320"/>
+        <c:crossAx val="62919808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51800320"/>
+        <c:axId val="62919808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1212,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51798784"/>
+        <c:crossAx val="62782848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1273,11 +1375,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51817472"/>
-        <c:axId val="54280960"/>
+        <c:axId val="62941056"/>
+        <c:axId val="62942592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51817472"/>
+        <c:axId val="62941056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,12 +1389,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54280960"/>
+        <c:crossAx val="62942592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54280960"/>
+        <c:axId val="62942592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1404,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51817472"/>
+        <c:crossAx val="62941056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1469,11 +1571,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54306304"/>
-        <c:axId val="54307840"/>
+        <c:axId val="62968576"/>
+        <c:axId val="62970112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54306304"/>
+        <c:axId val="62968576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1483,12 +1585,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54307840"/>
+        <c:crossAx val="62970112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54307840"/>
+        <c:axId val="62970112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1498,7 +1600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54306304"/>
+        <c:crossAx val="62968576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1671,11 +1773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="56552448"/>
-        <c:axId val="56550912"/>
+        <c:axId val="62809984"/>
+        <c:axId val="62811520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56552448"/>
+        <c:axId val="62809984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,12 +1787,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56550912"/>
+        <c:crossAx val="62811520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56550912"/>
+        <c:axId val="62811520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1700,7 +1802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56552448"/>
+        <c:crossAx val="62809984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3843,10 +3945,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Y18"/>
+  <dimension ref="B2:Z38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3865,23 +3967,31 @@
     <col min="25" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B2" s="51" t="s">
+    <row r="2" spans="2:26" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:25" s="40" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:26" s="40" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C5" s="40" t="s">
         <v>50</v>
       </c>
       <c r="J5" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="S5" s="40" t="s">
+      <c r="S5" s="62" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="2:25" s="39" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="63"/>
+      <c r="Y5" s="63"/>
+      <c r="Z5" s="64"/>
+    </row>
+    <row r="6" spans="2:26" s="39" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="39" t="s">
         <v>3</v>
       </c>
@@ -3927,29 +4037,30 @@
       <c r="Q6" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="39" t="s">
+      <c r="S6" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="T6" s="39" t="s">
+      <c r="T6" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="U6" s="39" t="s">
+      <c r="U6" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="V6" s="39" t="s">
+      <c r="V6" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="W6" s="39" t="s">
+      <c r="W6" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="X6" s="39" t="s">
+      <c r="X6" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="Y6" s="39" t="s">
+      <c r="Y6" s="55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z6" s="56"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -3988,31 +4099,32 @@
         <f>LN(P7)</f>
         <v>5.4380793089231956</v>
       </c>
-      <c r="S7" s="49">
+      <c r="S7" s="65">
         <v>2.5</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="52">
         <v>8780</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="52">
         <v>30</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="52">
         <v>30</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="52">
         <v>230</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="52">
         <f>(V7-U7)*W7</f>
         <v>0</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="52">
         <f>T7+X7</f>
         <v>8780</v>
       </c>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z7" s="53"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -4052,31 +4164,32 @@
         <f t="shared" ref="Q8:Q9" si="1">LN(P8)</f>
         <v>4.8675344504555822</v>
       </c>
-      <c r="S8" s="49">
+      <c r="S8" s="65">
         <v>5</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="52">
         <v>7790</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="52">
         <v>30</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="52">
         <v>30</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="52">
         <v>130</v>
       </c>
-      <c r="X8">
-        <f t="shared" ref="X8:X17" si="2">(V8-U8)*W8</f>
+      <c r="X8" s="52">
+        <f t="shared" ref="X8:X16" si="2">(V8-U8)*W8</f>
         <v>0</v>
       </c>
-      <c r="Y8">
-        <f t="shared" ref="Y8:Y17" si="3">T8+X8</f>
+      <c r="Y8" s="52">
+        <f t="shared" ref="Y8:Y15" si="3">T8+X8</f>
         <v>7790</v>
       </c>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z8" s="53"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -4111,7 +4224,7 @@
       <c r="M9">
         <v>40</v>
       </c>
-      <c r="N9" s="50">
+      <c r="N9" s="49">
         <v>50</v>
       </c>
       <c r="P9" s="47">
@@ -4121,31 +4234,32 @@
         <f t="shared" si="1"/>
         <v>4.3820266346738812</v>
       </c>
-      <c r="S9" s="49">
+      <c r="S9" s="65">
         <v>10</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="52">
         <v>7640</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="52">
         <v>33</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="52">
         <v>30</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="52">
         <v>80</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="52">
         <f t="shared" si="2"/>
         <v>-240</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="52">
         <f t="shared" si="3"/>
         <v>7400</v>
       </c>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z9" s="53"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -4176,7 +4290,7 @@
       <c r="M10">
         <v>40</v>
       </c>
-      <c r="N10" s="50">
+      <c r="N10" s="49">
         <v>50</v>
       </c>
       <c r="P10" s="43">
@@ -4184,31 +4298,32 @@
         <v>37.596549448771725</v>
       </c>
       <c r="Q10" s="45"/>
-      <c r="S10" s="49">
+      <c r="S10" s="65">
         <v>20</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="52">
         <v>7250</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="52">
         <v>37</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="52">
         <v>40</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="52">
         <v>37.596549448771725</v>
       </c>
-      <c r="X10">
+      <c r="X10" s="52">
         <f t="shared" si="2"/>
         <v>112.78964834631518</v>
       </c>
-      <c r="Y10">
+      <c r="Y10" s="52">
         <f t="shared" si="3"/>
         <v>7362.7896483463155</v>
       </c>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z10" s="53"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -4239,7 +4354,7 @@
       <c r="M11">
         <v>40</v>
       </c>
-      <c r="N11" s="50">
+      <c r="N11" s="49">
         <v>50</v>
       </c>
       <c r="P11" s="43">
@@ -4247,31 +4362,32 @@
         <v>16.421401516114997</v>
       </c>
       <c r="Q11" s="45"/>
-      <c r="S11" s="49">
+      <c r="S11" s="65">
         <v>50</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="52">
         <v>6400</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="52">
         <v>37</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="52">
         <v>40</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="52">
         <v>16.421401516114997</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="52">
         <f t="shared" si="2"/>
         <v>49.264204548344992</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="52">
         <f t="shared" si="3"/>
         <v>6449.2642045483453</v>
       </c>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z11" s="53"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -4313,31 +4429,32 @@
         <f>LN(P12)</f>
         <v>2.1282317058492679</v>
       </c>
-      <c r="S12" s="49">
+      <c r="S12" s="65">
         <v>100</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="52">
         <v>5370</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="52">
         <v>37</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="52">
         <v>40</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="52">
         <v>8.4</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="52">
         <f t="shared" si="2"/>
         <v>25.200000000000003</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="52">
         <f t="shared" si="3"/>
         <v>5395.2</v>
       </c>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z12" s="53"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -4360,31 +4477,32 @@
         <v>7.2939393877120153</v>
       </c>
       <c r="Q13" s="45"/>
-      <c r="S13" s="49">
+      <c r="S13" s="65">
         <v>250</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="52">
         <v>4037</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="52">
         <v>37</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="52">
         <v>50</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="52">
         <v>7.2939393877120153</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="52">
         <f t="shared" si="2"/>
         <v>94.821212040256199</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="52">
         <f t="shared" si="3"/>
         <v>4131.8212120402559</v>
       </c>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z13" s="53"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -4416,31 +4534,32 @@
         <v>6.5463839094293448</v>
       </c>
       <c r="Q14" s="45"/>
-      <c r="S14" s="49">
+      <c r="S14" s="65">
         <v>500</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="52">
         <v>3278</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="52">
         <v>50</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="52">
         <v>50</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="52">
         <v>6.5463839094293448</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" s="52">
         <f t="shared" si="3"/>
         <v>3278</v>
       </c>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z14" s="53"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -4473,31 +4592,32 @@
         <v>6.1451322566852165</v>
       </c>
       <c r="Q15" s="45"/>
-      <c r="S15" s="49">
+      <c r="S15" s="65">
         <v>750</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="52">
         <v>2480</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="52">
         <v>65</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="52">
         <v>50</v>
       </c>
-      <c r="W15">
+      <c r="W15" s="52">
         <v>6.1451322566852165</v>
       </c>
-      <c r="X15">
+      <c r="X15" s="52">
         <f t="shared" si="2"/>
         <v>-92.176983850278248</v>
       </c>
-      <c r="Y15">
+      <c r="Y15" s="52">
         <f t="shared" si="3"/>
         <v>2387.8230161497218</v>
       </c>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z15" s="53"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -4534,80 +4654,283 @@
         <f>LN(P16)</f>
         <v>1.7047480922384253</v>
       </c>
-      <c r="S16" s="52">
+      <c r="S16" s="65">
         <v>1000</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="52">
         <v>2145</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="52">
         <v>80</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="52">
         <v>80</v>
       </c>
-      <c r="W16" s="53">
+      <c r="W16" s="57">
         <v>5.8230000000000004</v>
       </c>
-      <c r="X16">
+      <c r="X16" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y16" s="54">
+      <c r="Y16" s="58">
         <f>T16</f>
         <v>2145</v>
       </c>
-    </row>
-    <row r="17" spans="19:25" x14ac:dyDescent="0.25">
-      <c r="S17" s="49">
+      <c r="Z16" s="53"/>
+    </row>
+    <row r="17" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S17" s="65">
         <v>1500</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="52">
         <v>1810</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="52">
         <v>80</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="52">
         <v>80</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="52">
         <v>5.5</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="52">
         <f>(V17-U17)*W17</f>
         <v>0</v>
       </c>
-      <c r="Y17">
+      <c r="Y17" s="52">
         <f>T17+X17</f>
         <v>1810</v>
       </c>
-    </row>
-    <row r="18" spans="19:25" x14ac:dyDescent="0.25">
-      <c r="S18" s="49">
+      <c r="Z17" s="53"/>
+    </row>
+    <row r="18" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S18" s="65">
         <f>3000</f>
         <v>3000</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="52">
         <v>1810</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="52">
         <v>80</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="52">
         <v>80</v>
       </c>
-      <c r="W18">
+      <c r="W18" s="52">
         <v>5.5</v>
       </c>
-      <c r="X18">
+      <c r="X18" s="52">
         <f>(V18-U18)*W18</f>
         <v>0</v>
       </c>
-      <c r="Y18">
+      <c r="Y18" s="52">
         <f>T18+X18</f>
         <v>1810</v>
       </c>
+      <c r="Z18" s="53"/>
+    </row>
+    <row r="19" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S19" s="51"/>
+      <c r="T19" s="52"/>
+      <c r="U19" s="52"/>
+      <c r="V19" s="52"/>
+      <c r="W19" s="52"/>
+      <c r="X19" s="52"/>
+      <c r="Y19" s="52"/>
+      <c r="Z19" s="53"/>
+    </row>
+    <row r="20" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S20" s="51"/>
+      <c r="T20" s="52"/>
+      <c r="U20" s="52"/>
+      <c r="V20" s="52"/>
+      <c r="W20" s="52"/>
+      <c r="X20" s="52"/>
+      <c r="Y20" s="52"/>
+      <c r="Z20" s="53"/>
+    </row>
+    <row r="21" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S21" s="51"/>
+      <c r="T21" s="52"/>
+      <c r="U21" s="52"/>
+      <c r="V21" s="52"/>
+      <c r="W21" s="52"/>
+      <c r="X21" s="52"/>
+      <c r="Y21" s="52"/>
+      <c r="Z21" s="53"/>
+    </row>
+    <row r="22" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S22" s="51"/>
+      <c r="T22" s="52"/>
+      <c r="U22" s="52"/>
+      <c r="V22" s="52"/>
+      <c r="W22" s="52"/>
+      <c r="X22" s="52"/>
+      <c r="Y22" s="52"/>
+      <c r="Z22" s="53"/>
+    </row>
+    <row r="23" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S23" s="51"/>
+      <c r="T23" s="52"/>
+      <c r="U23" s="52"/>
+      <c r="V23" s="52"/>
+      <c r="W23" s="52"/>
+      <c r="X23" s="52"/>
+      <c r="Y23" s="52"/>
+      <c r="Z23" s="53"/>
+    </row>
+    <row r="24" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S24" s="51"/>
+      <c r="T24" s="52"/>
+      <c r="U24" s="52"/>
+      <c r="V24" s="52"/>
+      <c r="W24" s="52"/>
+      <c r="X24" s="52"/>
+      <c r="Y24" s="52"/>
+      <c r="Z24" s="53"/>
+    </row>
+    <row r="25" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S25" s="51"/>
+      <c r="T25" s="52"/>
+      <c r="U25" s="52"/>
+      <c r="V25" s="52"/>
+      <c r="W25" s="52"/>
+      <c r="X25" s="52"/>
+      <c r="Y25" s="52"/>
+      <c r="Z25" s="53"/>
+    </row>
+    <row r="26" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S26" s="51"/>
+      <c r="T26" s="52"/>
+      <c r="U26" s="52"/>
+      <c r="V26" s="52"/>
+      <c r="W26" s="52"/>
+      <c r="X26" s="52"/>
+      <c r="Y26" s="52"/>
+      <c r="Z26" s="53"/>
+    </row>
+    <row r="27" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S27" s="51"/>
+      <c r="T27" s="52"/>
+      <c r="U27" s="52"/>
+      <c r="V27" s="52"/>
+      <c r="W27" s="52"/>
+      <c r="X27" s="52"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="53"/>
+    </row>
+    <row r="28" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S28" s="51"/>
+      <c r="T28" s="52"/>
+      <c r="U28" s="52"/>
+      <c r="V28" s="52"/>
+      <c r="W28" s="52"/>
+      <c r="X28" s="52"/>
+      <c r="Y28" s="52"/>
+      <c r="Z28" s="53"/>
+    </row>
+    <row r="29" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S29" s="51"/>
+      <c r="T29" s="52"/>
+      <c r="U29" s="52"/>
+      <c r="V29" s="52"/>
+      <c r="W29" s="52"/>
+      <c r="X29" s="52"/>
+      <c r="Y29" s="52"/>
+      <c r="Z29" s="53"/>
+    </row>
+    <row r="30" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S30" s="51"/>
+      <c r="T30" s="52"/>
+      <c r="U30" s="52"/>
+      <c r="V30" s="52"/>
+      <c r="W30" s="52"/>
+      <c r="X30" s="52"/>
+      <c r="Y30" s="52"/>
+      <c r="Z30" s="53"/>
+    </row>
+    <row r="31" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S31" s="51"/>
+      <c r="T31" s="52"/>
+      <c r="U31" s="52"/>
+      <c r="V31" s="52"/>
+      <c r="W31" s="52"/>
+      <c r="X31" s="52"/>
+      <c r="Y31" s="52"/>
+      <c r="Z31" s="53"/>
+    </row>
+    <row r="32" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S32" s="51"/>
+      <c r="T32" s="52"/>
+      <c r="U32" s="52"/>
+      <c r="V32" s="52"/>
+      <c r="W32" s="52"/>
+      <c r="X32" s="52"/>
+      <c r="Y32" s="52"/>
+      <c r="Z32" s="53"/>
+    </row>
+    <row r="33" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S33" s="51"/>
+      <c r="T33" s="52"/>
+      <c r="U33" s="52"/>
+      <c r="V33" s="52"/>
+      <c r="W33" s="52"/>
+      <c r="X33" s="52"/>
+      <c r="Y33" s="52"/>
+      <c r="Z33" s="53"/>
+    </row>
+    <row r="34" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S34" s="51"/>
+      <c r="T34" s="52"/>
+      <c r="U34" s="52"/>
+      <c r="V34" s="52"/>
+      <c r="W34" s="52"/>
+      <c r="X34" s="52"/>
+      <c r="Y34" s="52"/>
+      <c r="Z34" s="53"/>
+    </row>
+    <row r="35" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S35" s="51"/>
+      <c r="T35" s="52"/>
+      <c r="U35" s="52"/>
+      <c r="V35" s="52"/>
+      <c r="W35" s="52"/>
+      <c r="X35" s="52"/>
+      <c r="Y35" s="52"/>
+      <c r="Z35" s="53"/>
+    </row>
+    <row r="36" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S36" s="51"/>
+      <c r="T36" s="52"/>
+      <c r="U36" s="52"/>
+      <c r="V36" s="52"/>
+      <c r="W36" s="52"/>
+      <c r="X36" s="52"/>
+      <c r="Y36" s="52"/>
+      <c r="Z36" s="53"/>
+    </row>
+    <row r="37" spans="19:26" x14ac:dyDescent="0.25">
+      <c r="S37" s="51"/>
+      <c r="T37" s="52"/>
+      <c r="U37" s="52"/>
+      <c r="V37" s="52"/>
+      <c r="W37" s="52"/>
+      <c r="X37" s="52"/>
+      <c r="Y37" s="52"/>
+      <c r="Z37" s="53"/>
+    </row>
+    <row r="38" spans="19:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S38" s="59"/>
+      <c r="T38" s="60"/>
+      <c r="U38" s="60"/>
+      <c r="V38" s="60"/>
+      <c r="W38" s="60"/>
+      <c r="X38" s="60"/>
+      <c r="Y38" s="60"/>
+      <c r="Z38" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>